<commit_message>
User stories updated + Kanban link added
</commit_message>
<xml_diff>
--- a/Deneuville_Fabian_2_user_stories_032023.xlsx
+++ b/Deneuville_Fabian_2_user_stories_032023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabiandeneuville/Documents/FORMATION/OPEN CLASSROOMS - REACT/PROJETS/FabianDeneuville_10_03032023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1422F985-8C7C-F64C-AA55-1964B1212DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D50528-0D48-9F43-8252-04BDC5343F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0DA559FF-AC57-D343-8D5A-67E81EC7576A}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{0DA559FF-AC57-D343-8D5A-67E81EC7576A}"/>
   </bookViews>
   <sheets>
     <sheet name="Inscription" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="109">
   <si>
     <t>INSCRIPTION</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Je suis un utilisateur (pédagogue ou élève) pas encore inscrit sur l'application et j'arrive sur la page d'inscription.</t>
   </si>
   <si>
-    <t>Je reçois un mail pour confirmer mon inscription. Je suis inscrit et suis redirigé vers le tableau de bord mais ne peux pas encore interagir avec tant que je n'ai validé mon inscription.</t>
-  </si>
-  <si>
     <t>J'ai procédé à mon inscription et ai reçu le mail de confirmation.</t>
   </si>
   <si>
@@ -296,6 +293,57 @@
   </si>
   <si>
     <t>Je peux visualiser l'ensemble de mes évènements, ainsi que l'élève associé. Les évènements liés à des élèves pour lesquels les élèves ont demandé la suppression ou une modification sont mis en évidence. Je peux valider ou non ces demandes.</t>
+  </si>
+  <si>
+    <t>J'accède à la liste des tâches depuis le dashboard.</t>
+  </si>
+  <si>
+    <t>Je suis un utilisateur connecté (pédagogue ou élève) ayant déjà créé des tâches.</t>
+  </si>
+  <si>
+    <t>Je suis un utilisateur connecté (pédagogue ou élève) n'ayant jamais créé de tâches.</t>
+  </si>
+  <si>
+    <t>Un message m'informe que je n'ai encore créé aucune tâche. Le formulaire de création de tâche est ouvert.</t>
+  </si>
+  <si>
+    <t>Je visualise l'ensemble de mes tâches sous forme de liste. Les tâches non réalisées ayant la deadline la plus proche apparaissent en tête de liste. Un formulaire de création de tâche peut être ouvert pour ajouter une tâche.</t>
+  </si>
+  <si>
+    <t>Je peux voir les tâches qui m'ont été assignées par un professeur.</t>
+  </si>
+  <si>
+    <t>J'accède à la liste de mes élèves depuis le dashboard.</t>
+  </si>
+  <si>
+    <t>Je peux accéder à la liste des tâches de chaque élève et ajouter des tâches.</t>
+  </si>
+  <si>
+    <t>9. Scénario nominal</t>
+  </si>
+  <si>
+    <t>Je suis un pédagioogue connecté.</t>
+  </si>
+  <si>
+    <t>Je me trouve sur le dashboard. La liste des mes élèves est affichée. Je clique sur un élève de la liste.</t>
+  </si>
+  <si>
+    <t>Je suis redirigé par la liste des tâches de l'élève.</t>
+  </si>
+  <si>
+    <t>Je suis sur la page de la liste des tâches.</t>
+  </si>
+  <si>
+    <t>Je peux ajouter une nouvelle tâche.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je peux changer le statut d'une tâche (en cours -&gt; complétée) </t>
+  </si>
+  <si>
+    <t>Je peux supprimer une tâche de ma propre liste ou les tâches que j'ai moi-même créé dans la liste d'un élève.</t>
+  </si>
+  <si>
+    <t>Je peux supprimer une tâche que j'ai moi-même créé.</t>
   </si>
   <si>
     <r>
@@ -404,59 +452,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>ainsi que la ou les matières pour lesquelles je souhaite apporter ou recevoir de l'aide puis je clique sur le bouton de soummission du formulaire.</t>
+      <t>ainsi que la ou les matières pour lesquelles je souhaite apporter ou recevoir de l'aide puis je clique sur le bouton de soumission du formulaire.</t>
     </r>
   </si>
   <si>
-    <t>J'accède à la liste des tâches depuis le dashboard.</t>
-  </si>
-  <si>
-    <t>Je suis un utilisateur connecté (pédagogue ou élève) ayant déjà créé des tâches.</t>
-  </si>
-  <si>
-    <t>Je suis un utilisateur connecté (pédagogue ou élève) n'ayant jamais créé de tâches.</t>
-  </si>
-  <si>
-    <t>Un message m'informe que je n'ai encore créé aucune tâche. Le formulaire de création de tâche est ouvert.</t>
-  </si>
-  <si>
-    <t>Je visualise l'ensemble de mes tâches sous forme de liste. Les tâches non réalisées ayant la deadline la plus proche apparaissent en tête de liste. Un formulaire de création de tâche peut être ouvert pour ajouter une tâche.</t>
-  </si>
-  <si>
-    <t>Je peux voir les tâches qui m'ont été assignées par un professeur.</t>
-  </si>
-  <si>
-    <t>J'accède à la liste de mes élèves depuis le dashboard.</t>
-  </si>
-  <si>
-    <t>Je peux accéder à la liste des tâches de chaque élève et ajouter des tâches.</t>
-  </si>
-  <si>
-    <t>9. Scénario nominal</t>
-  </si>
-  <si>
-    <t>Je suis un pédagioogue connecté.</t>
-  </si>
-  <si>
-    <t>Je me trouve sur le dashboard. La liste des mes élèves est affichée. Je clique sur un élève de la liste.</t>
-  </si>
-  <si>
-    <t>Je suis redirigé par la liste des tâches de l'élève.</t>
-  </si>
-  <si>
-    <t>Je suis sur la page de la liste des tâches.</t>
-  </si>
-  <si>
-    <t>Je peux ajouter une nouvelle tâche.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je peux changer le statut d'une tâche (en cours -&gt; complétée) </t>
-  </si>
-  <si>
-    <t>Je peux supprimer une tâche de ma propre liste ou les tâches que j'ai moi-même créé dans la liste d'un élève.</t>
-  </si>
-  <si>
-    <t>Je peux supprimer une tâche que j'ai moi-même créé.</t>
+    <t>Je reçois un mail pour confirmer mon inscription. Je suis inscrit et suis redirigé vers le tableau de bord mais ne peux pas encore interagir avec tant que je n'ai pas validé mon inscription.</t>
+  </si>
+  <si>
+    <t>3. Scénario alternatif</t>
+  </si>
+  <si>
+    <t>Je peux entamer une conversation en envoyant un premier message.</t>
+  </si>
+  <si>
+    <t>Je recherche un pédagogue.</t>
+  </si>
+  <si>
+    <t>Je suis un pédagogue connecté. J'ai accédé à la messagerie depuis le dashboard.</t>
+  </si>
+  <si>
+    <t>Je peux voir les conversations ouvertes par des élèves me concernant. Je clique sur l'une d'elle.</t>
+  </si>
+  <si>
+    <t>J'arrive sur la conversation et peux répondre à l'élève.</t>
   </si>
 </sst>
 </file>
@@ -598,7 +616,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -712,6 +730,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,7 +1056,7 @@
   <dimension ref="A2:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,26 +1107,26 @@
       <c r="P3" s="20"/>
     </row>
     <row r="4" spans="1:16" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
+      <c r="A4" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+      <c r="P4" s="37"/>
     </row>
     <row r="5" spans="1:16" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
@@ -1137,7 +1159,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1149,7 +1171,7 @@
         <v>7</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
@@ -1163,7 +1185,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="C7" s="23"/>
       <c r="D7" s="23"/>
@@ -1175,7 +1197,7 @@
         <v>8</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K7" s="19"/>
       <c r="L7" s="19"/>
@@ -1185,33 +1207,33 @@
       <c r="P7" s="19"/>
     </row>
     <row r="8" spans="1:16" ht="21" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
+      <c r="A8" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="37"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
     </row>
     <row r="9" spans="1:16" s="6" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1223,7 +1245,7 @@
         <v>6</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
@@ -1237,7 +1259,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1249,7 +1271,7 @@
         <v>7</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
@@ -1263,7 +1285,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="19"/>
@@ -1275,7 +1297,7 @@
         <v>8</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="K11" s="19"/>
       <c r="L11" s="19"/>
@@ -1359,7 +1381,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="I7" sqref="I7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1410,7 +1432,7 @@
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1419,23 +1441,23 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="I3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1447,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
@@ -1461,7 +1483,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1473,7 +1495,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
@@ -1487,7 +1509,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1499,7 +1521,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
@@ -1510,7 +1532,7 @@
     </row>
     <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -1519,23 +1541,23 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
+      <c r="I7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1547,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
@@ -1561,7 +1583,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1573,7 +1595,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
@@ -1587,7 +1609,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1599,7 +1621,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
@@ -1637,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F8010C4-7E2A-3547-9649-1BAF3668A177}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7:P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1689,7 +1711,7 @@
     </row>
     <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1698,23 +1720,23 @@
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
-      <c r="I3" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
+      <c r="I3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -1726,7 +1748,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K4" s="22"/>
       <c r="L4" s="22"/>
@@ -1740,7 +1762,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="23"/>
@@ -1752,7 +1774,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
@@ -1766,7 +1788,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -1778,7 +1800,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="19"/>
       <c r="L6" s="19"/>
@@ -1789,7 +1811,7 @@
     </row>
     <row r="7" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
@@ -1798,23 +1820,23 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
+      <c r="I7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" ht="43" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="19"/>
@@ -1826,7 +1848,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="19"/>
       <c r="L8" s="19"/>
@@ -1840,7 +1862,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="19"/>
@@ -1852,7 +1874,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K9" s="19"/>
       <c r="L9" s="19"/>
@@ -1866,7 +1888,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
@@ -1878,7 +1900,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
@@ -1889,7 +1911,7 @@
     </row>
     <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -1912,7 +1934,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -1934,7 +1956,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -1956,7 +1978,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
@@ -1975,7 +1997,7 @@
     </row>
     <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -1998,7 +2020,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
@@ -2020,7 +2042,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
@@ -2042,7 +2064,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
@@ -2061,7 +2083,7 @@
     </row>
     <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -2084,7 +2106,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -2106,7 +2128,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -2128,7 +2150,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -2147,7 +2169,7 @@
     </row>
     <row r="23" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -2170,7 +2192,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="19"/>
       <c r="D24" s="19"/>
@@ -2192,7 +2214,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -2214,7 +2236,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -2233,7 +2255,7 @@
     </row>
     <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -2256,7 +2278,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -2278,7 +2300,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -2300,7 +2322,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -2319,7 +2341,7 @@
     </row>
     <row r="31" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2342,7 +2364,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -2364,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -2386,7 +2408,7 @@
         <v>8</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -2405,7 +2427,7 @@
     </row>
     <row r="35" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -2428,7 +2450,7 @@
         <v>6</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -2450,7 +2472,7 @@
         <v>7</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -2472,7 +2494,7 @@
         <v>8</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -2572,10 +2594,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E8922CE-E80E-CA4D-AB87-6E9B058A0049}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:H10"/>
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18:P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2626,7 +2648,7 @@
     </row>
     <row r="3" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -2635,23 +2657,23 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
-      <c r="I3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="I3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -2663,7 +2685,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
@@ -2677,7 +2699,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -2689,7 +2711,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="26" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
@@ -2703,7 +2725,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -2715,7 +2737,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
@@ -2726,7 +2748,7 @@
     </row>
     <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -2735,16 +2757,16 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
+      <c r="I7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
@@ -2763,7 +2785,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -2777,7 +2799,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -2789,7 +2811,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>42</v>
+        <v>107</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
@@ -2803,7 +2825,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>46</v>
+        <v>104</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -2811,11 +2833,11 @@
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="8" t="s">
+      <c r="I10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
@@ -2824,9 +2846,9 @@
       <c r="O10" s="26"/>
       <c r="P10" s="26"/>
     </row>
-    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -2835,21 +2857,23 @@
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
       <c r="H11" s="28"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="29"/>
-      <c r="L11" s="29"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="29"/>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-    </row>
-    <row r="12" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I11" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+    </row>
+    <row r="12" spans="1:16" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
@@ -2857,21 +2881,25 @@
       <c r="F12" s="26"/>
       <c r="G12" s="26"/>
       <c r="H12" s="26"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-    </row>
-    <row r="13" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I12" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="J12" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+    </row>
+    <row r="13" spans="1:16" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -2879,21 +2907,25 @@
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="31"/>
-      <c r="M13" s="31"/>
-      <c r="N13" s="31"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-    </row>
-    <row r="14" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="30"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="30"/>
+    </row>
+    <row r="14" spans="1:16" s="10" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
@@ -2901,18 +2933,22 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="H14" s="26"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-      <c r="M14" s="27"/>
-      <c r="N14" s="27"/>
-      <c r="O14" s="27"/>
-      <c r="P14" s="27"/>
+      <c r="I14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
     </row>
     <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -2935,7 +2971,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -2944,20 +2980,20 @@
       <c r="G16" s="26"/>
       <c r="H16" s="26"/>
       <c r="I16" s="16"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="27"/>
-      <c r="O16" s="27"/>
-      <c r="P16" s="27"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="38"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="38"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
+      <c r="P16" s="38"/>
     </row>
     <row r="17" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -2979,7 +3015,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -2998,7 +3034,7 @@
     </row>
     <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -3021,7 +3057,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -3043,7 +3079,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -3065,7 +3101,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C22" s="26"/>
       <c r="D22" s="26"/>
@@ -3082,49 +3118,142 @@
       <c r="O22" s="27"/>
       <c r="P22" s="27"/>
     </row>
+    <row r="23" spans="1:16" ht="21" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+    </row>
+    <row r="24" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="27"/>
+      <c r="N24" s="27"/>
+      <c r="O24" s="27"/>
+      <c r="P24" s="27"/>
+    </row>
+    <row r="25" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="31"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
+      <c r="N25" s="31"/>
+      <c r="O25" s="31"/>
+      <c r="P25" s="31"/>
+    </row>
+    <row r="26" spans="1:16" s="10" customFormat="1" ht="46" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+      <c r="M26" s="27"/>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+    </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="48">
     <mergeCell ref="A1:P2"/>
     <mergeCell ref="A3:H3"/>
     <mergeCell ref="I3:P3"/>
     <mergeCell ref="B4:H4"/>
-    <mergeCell ref="J4:P4"/>
     <mergeCell ref="B5:H5"/>
     <mergeCell ref="J5:P5"/>
     <mergeCell ref="B6:H6"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="I11:P11"/>
+    <mergeCell ref="J6:P6"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="I7:P7"/>
-    <mergeCell ref="J6:P6"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="I11:P11"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="J12:P12"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="J8:P8"/>
     <mergeCell ref="B9:H9"/>
     <mergeCell ref="J9:P9"/>
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="J10:P10"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="I15:P15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="J4:P4"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="J12:P12"/>
     <mergeCell ref="B13:H13"/>
     <mergeCell ref="J13:P13"/>
     <mergeCell ref="B14:H14"/>
     <mergeCell ref="J14:P14"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="I15:P15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="J16:P16"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="J17:P17"/>
     <mergeCell ref="B18:H18"/>
     <mergeCell ref="J18:P18"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="J22:P22"/>
     <mergeCell ref="A19:H19"/>
     <mergeCell ref="I19:P19"/>
     <mergeCell ref="B20:H20"/>
     <mergeCell ref="J20:P20"/>
     <mergeCell ref="B21:H21"/>
     <mergeCell ref="J21:P21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="J22:P22"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="J26:P26"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="I23:P23"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="J24:P24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="J25:P25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -3135,8 +3264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FE9BFE0-07A2-9F4A-A52F-77D27DF4B376}">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3187,7 +3316,7 @@
     </row>
     <row r="3" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -3210,7 +3339,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -3232,7 +3361,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -3254,7 +3383,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -3273,7 +3402,7 @@
     </row>
     <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -3282,23 +3411,23 @@
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
       <c r="H7" s="28"/>
-      <c r="I7" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="J7" s="29"/>
-      <c r="K7" s="29"/>
-      <c r="L7" s="29"/>
-      <c r="M7" s="29"/>
-      <c r="N7" s="29"/>
-      <c r="O7" s="29"/>
-      <c r="P7" s="29"/>
+      <c r="I7" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
     </row>
     <row r="8" spans="1:16" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="26"/>
       <c r="D8" s="26"/>
@@ -3310,7 +3439,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
@@ -3324,7 +3453,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -3336,7 +3465,7 @@
         <v>7</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
@@ -3350,7 +3479,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -3362,7 +3491,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
@@ -3373,7 +3502,7 @@
     </row>
     <row r="11" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -3396,7 +3525,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C12" s="26"/>
       <c r="D12" s="26"/>
@@ -3418,7 +3547,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -3440,7 +3569,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C14" s="26"/>
       <c r="D14" s="26"/>
@@ -3459,7 +3588,7 @@
     </row>
     <row r="15" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -3482,7 +3611,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="26"/>
       <c r="D16" s="26"/>
@@ -3504,7 +3633,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -3526,7 +3655,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="26"/>
       <c r="D18" s="26"/>
@@ -3589,7 +3718,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="I3" sqref="I3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3640,7 +3769,7 @@
     </row>
     <row r="3" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
@@ -3649,23 +3778,23 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
       <c r="H3" s="28"/>
-      <c r="I3" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="I3" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
     </row>
     <row r="4" spans="1:16" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
@@ -3677,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="J4" s="33" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
@@ -3691,7 +3820,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -3703,7 +3832,7 @@
         <v>7</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
@@ -3712,12 +3841,12 @@
       <c r="O5" s="30"/>
       <c r="P5" s="30"/>
     </row>
-    <row r="6" spans="1:16" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" s="10" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="30"/>
       <c r="D6" s="30"/>
@@ -3729,7 +3858,7 @@
         <v>8</v>
       </c>
       <c r="J6" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
@@ -3740,7 +3869,7 @@
     </row>
     <row r="7" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="28"/>
       <c r="C7" s="28"/>
@@ -3763,7 +3892,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C8" s="33"/>
       <c r="D8" s="33"/>
@@ -3785,7 +3914,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="30"/>
@@ -3807,7 +3936,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="26"/>
@@ -3826,7 +3955,7 @@
     </row>
     <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="28"/>
@@ -3849,7 +3978,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="33"/>
@@ -3871,7 +4000,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="30" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="30"/>
@@ -3893,7 +4022,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="30"/>
       <c r="D14" s="30"/>
@@ -3912,7 +4041,7 @@
     </row>
     <row r="15" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -3935,7 +4064,7 @@
         <v>6</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="33"/>
       <c r="D16" s="33"/>
@@ -3957,7 +4086,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
@@ -3979,7 +4108,7 @@
         <v>8</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
@@ -3998,7 +4127,7 @@
     </row>
     <row r="19" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A19" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -4021,7 +4150,7 @@
         <v>6</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="33"/>
@@ -4043,7 +4172,7 @@
         <v>7</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
@@ -4065,7 +4194,7 @@
         <v>8</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
@@ -4084,7 +4213,7 @@
     </row>
     <row r="23" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A23" s="28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="28"/>
       <c r="C23" s="28"/>
@@ -4107,7 +4236,7 @@
         <v>6</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="33"/>
       <c r="D24" s="33"/>
@@ -4129,7 +4258,7 @@
         <v>7</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="30"/>
@@ -4151,7 +4280,7 @@
         <v>8</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C26" s="30"/>
       <c r="D26" s="30"/>
@@ -4170,7 +4299,7 @@
     </row>
     <row r="27" spans="1:16" ht="21" x14ac:dyDescent="0.2">
       <c r="A27" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="28"/>
       <c r="C27" s="28"/>
@@ -4193,7 +4322,7 @@
         <v>6</v>
       </c>
       <c r="B28" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="33"/>
       <c r="D28" s="33"/>
@@ -4215,7 +4344,7 @@
         <v>7</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="30"/>
@@ -4237,7 +4366,7 @@
         <v>8</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>

</xml_diff>